<commit_message>
update to environmental data summary
</commit_message>
<xml_diff>
--- a/data/environment/annualized_env_data.xlsx
+++ b/data/environment/annualized_env_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
   <si>
     <t>Year</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -171,13 +168,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -547,8 +544,12 @@
       <c r="V2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
+      <c r="W2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
     </row>
@@ -2042,8 +2043,8 @@
       <c r="O22" s="7">
         <v>105.664</v>
       </c>
-      <c r="P22" s="3">
-        <v>0.987099874</v>
+      <c r="P22" s="9">
+        <v>1.110639</v>
       </c>
       <c r="Q22" s="3">
         <v>0.17</v>
@@ -2118,8 +2119,8 @@
       <c r="O23" s="7">
         <v>250.698</v>
       </c>
-      <c r="P23" s="3">
-        <v>1.014625661</v>
+      <c r="P23" s="7">
+        <v>1.003967</v>
       </c>
       <c r="Q23" s="3">
         <v>0.0</v>
@@ -2194,8 +2195,8 @@
       <c r="O24" s="7">
         <v>96.266</v>
       </c>
-      <c r="P24" s="3">
-        <v>0.970888898</v>
+      <c r="P24" s="7">
+        <v>0.954683</v>
       </c>
       <c r="Q24" s="3">
         <v>0.035</v>
@@ -2270,8 +2271,8 @@
       <c r="O25" s="7">
         <v>262.636</v>
       </c>
-      <c r="P25" s="3">
-        <v>1.068043951</v>
+      <c r="P25" s="7">
+        <v>1.101314</v>
       </c>
       <c r="Q25" s="3">
         <v>0.11</v>
@@ -2346,8 +2347,8 @@
       <c r="O26" s="7">
         <v>145.542</v>
       </c>
-      <c r="P26" s="3">
-        <v>1.009905749</v>
+      <c r="P26" s="7">
+        <v>1.019847</v>
       </c>
       <c r="Q26" s="3">
         <v>-0.4025</v>
@@ -2422,8 +2423,8 @@
       <c r="O27" s="7">
         <v>137.16</v>
       </c>
-      <c r="P27" s="3">
-        <v>0.952075054</v>
+      <c r="P27" s="7">
+        <v>0.987426</v>
       </c>
       <c r="Q27" s="3">
         <v>-0.3275</v>
@@ -2498,8 +2499,8 @@
       <c r="O28" s="7">
         <v>237.744</v>
       </c>
-      <c r="P28" s="3">
-        <v>1.058661781</v>
+      <c r="P28" s="7">
+        <v>0.987383</v>
       </c>
       <c r="Q28" s="3">
         <v>-0.7</v>
@@ -2574,8 +2575,8 @@
       <c r="O29" s="7">
         <v>264.414</v>
       </c>
-      <c r="P29" s="3">
-        <v>1.053676479</v>
+      <c r="P29" s="7">
+        <v>1.023238</v>
       </c>
       <c r="Q29" s="3">
         <v>-0.51</v>
@@ -2650,8 +2651,8 @@
       <c r="O30" s="7">
         <v>113.538</v>
       </c>
-      <c r="P30" s="3">
-        <v>1.074643222</v>
+      <c r="P30" s="7">
+        <v>1.086659</v>
       </c>
       <c r="Q30" s="3">
         <v>-0.8125</v>
@@ -2726,8 +2727,8 @@
       <c r="O31" s="7">
         <v>213.106</v>
       </c>
-      <c r="P31" s="3">
-        <v>1.028567984</v>
+      <c r="P31" s="7">
+        <v>1.095286</v>
       </c>
       <c r="Q31" s="3">
         <v>-0.9</v>
@@ -2802,8 +2803,8 @@
       <c r="O32" s="7">
         <v>71.12</v>
       </c>
-      <c r="P32" s="3">
-        <v>1.003547109</v>
+      <c r="P32" s="7">
+        <v>0.947779</v>
       </c>
       <c r="Q32" s="3">
         <v>-1.355</v>
@@ -2878,8 +2879,8 @@
       <c r="O33" s="7">
         <v>191.516</v>
       </c>
-      <c r="P33" s="3">
-        <v>0.990723096</v>
+      <c r="P33" s="7">
+        <v>1.146537</v>
       </c>
       <c r="Q33" s="3">
         <v>0.6</v>
@@ -2954,8 +2955,8 @@
       <c r="O34" s="7">
         <v>198.628</v>
       </c>
-      <c r="P34" s="3">
-        <v>1.0458818</v>
+      <c r="P34" s="7">
+        <v>0.952756</v>
       </c>
       <c r="Q34" s="3">
         <v>-0.2125</v>
@@ -3030,8 +3031,8 @@
       <c r="O35" s="7">
         <v>294.386</v>
       </c>
-      <c r="P35" s="3">
-        <v>1.00061507</v>
+      <c r="P35" s="7">
+        <v>1.038843</v>
       </c>
       <c r="Q35" s="3">
         <v>-1.165</v>
@@ -3106,8 +3107,8 @@
       <c r="O36" s="7">
         <v>113.03</v>
       </c>
-      <c r="P36" s="3">
-        <v>1.045679475</v>
+      <c r="P36" s="7">
+        <v>1.070438</v>
       </c>
       <c r="Q36" s="3">
         <v>-0.8075</v>
@@ -3182,8 +3183,8 @@
       <c r="O37" s="7">
         <v>196.596</v>
       </c>
-      <c r="P37" s="3">
-        <v>1.091835083</v>
+      <c r="P37" s="7">
+        <v>1.067878</v>
       </c>
       <c r="Q37" s="3">
         <v>-0.1</v>
@@ -3258,8 +3259,8 @@
       <c r="O38" s="7">
         <v>176.022</v>
       </c>
-      <c r="P38" s="3">
-        <v>1.03764974</v>
+      <c r="P38" s="7">
+        <v>1.086298</v>
       </c>
       <c r="Q38" s="3">
         <v>1.53</v>
@@ -3268,7 +3269,7 @@
         <v>0.7425</v>
       </c>
       <c r="S38" s="7">
-        <v>0.51</v>
+        <v>0.6258333</v>
       </c>
       <c r="T38" s="5">
         <v>8.057</v>
@@ -3301,22 +3302,22 @@
       <c r="D39" s="7">
         <v>1.217163</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="10">
         <v>17.25344</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="10">
         <v>0.22064</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="10">
         <v>1.85228</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="10">
         <v>5.097408</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="10">
         <v>0.86833</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="10">
         <v>0.23933</v>
       </c>
       <c r="K39" s="7">
@@ -3334,17 +3335,17 @@
       <c r="O39" s="7">
         <v>108.966</v>
       </c>
-      <c r="P39" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q39" s="9">
-        <v>-0.9616</v>
-      </c>
-      <c r="R39" s="3">
-        <v>0.6818</v>
-      </c>
-      <c r="S39" s="9">
-        <v>-0.3184</v>
+      <c r="P39" s="7">
+        <v>0.967345</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>-0.963</v>
+      </c>
+      <c r="R39" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="S39" s="7">
+        <v>0.6258333</v>
       </c>
       <c r="T39" s="11"/>
       <c r="U39" s="11"/>
@@ -3388,10 +3389,18 @@
       <c r="O40" s="7">
         <v>96.012</v>
       </c>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
+      <c r="P40" s="7">
+        <v>1.047394</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>-0.07</v>
+      </c>
+      <c r="R40" s="7">
+        <v>1.2025</v>
+      </c>
+      <c r="S40" s="7">
+        <v>-0.133333</v>
+      </c>
       <c r="T40" s="11"/>
       <c r="U40" s="11"/>
       <c r="V40" s="7">

</xml_diff>